<commit_message>
chup man hinh update test loi
</commit_message>
<xml_diff>
--- a/testting/bang_test_loi.xlsx
+++ b/testting/bang_test_loi.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
   <si>
     <t>STT</t>
   </si>
@@ -100,6 +100,33 @@
   </si>
   <si>
     <t>xuất excel chi nhánh không đúng theo kết quả lọc</t>
+  </si>
+  <si>
+    <t>không cho tùy chỉnh loại khách hàng lúc thêm, edit</t>
+  </si>
+  <si>
+    <t>lúc thêm mặc định là khách lẻ</t>
+  </si>
+  <si>
+    <t>header chi tiết phiếu nhập nên để là mã chứng từ thay cho id</t>
+  </si>
+  <si>
+    <t>trong chi tiet phieu nhap thieu thong tin nha cung cap</t>
+  </si>
+  <si>
+    <t>xuất file excel danh sách chi nhánh trong module nhập xuất chưa hoàn chỉnh</t>
+  </si>
+  <si>
+    <t>báo cáo doanh thu theo chi nhánh: phần chọn tất cả chi nhánh hình như chưa làm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nếu rảnh </t>
+  </si>
+  <si>
+    <t>báo cáo: chỉnh header thể hiện biễu đồ đang biễu diễn về sản phẩm j, chi nhánh nào…</t>
+  </si>
+  <si>
+    <t>tắt hiển thị phần thao tác trong phân quyền</t>
   </si>
 </sst>
 </file>
@@ -201,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -224,6 +251,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -518,16 +548,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="2" width="60.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="74.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.85546875" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="58.140625" bestFit="1" customWidth="1"/>
@@ -732,7 +762,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:5">
       <c r="A17" s="7">
         <v>16</v>
       </c>
@@ -740,12 +770,74 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:5">
       <c r="A18" s="7">
         <v>17</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="10">
+        <v>18</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="10">
+        <v>19</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="10">
+        <v>20</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="10">
+        <v>21</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="10">
+        <v>22</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="10">
+        <v>23</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="10">
+        <v>24</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>